<commit_message>
Seventh commit 20th april 6.20pm
</commit_message>
<xml_diff>
--- a/Project Flow.xlsx
+++ b/Project Flow.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
   <si>
     <t xml:space="preserve">Login Page </t>
   </si>
@@ -123,18 +123,6 @@
     <t xml:space="preserve">varchar(100) </t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0 = Inactive  </t>
-  </si>
-  <si>
-    <t>1=active</t>
-  </si>
-  <si>
     <t>ItemName</t>
   </si>
   <si>
@@ -147,27 +135,9 @@
     <t>Foreign Key reference (EventId)Events</t>
   </si>
   <si>
-    <t>Ratings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(From 1 to 10 scale) </t>
-  </si>
-  <si>
-    <t>PSNO</t>
-  </si>
-  <si>
     <t>Foreign key references (PSNO)Users</t>
   </si>
   <si>
-    <t>ItemNumber</t>
-  </si>
-  <si>
-    <t>Foreign key references (ItemNumber)Ideas</t>
-  </si>
-  <si>
     <t>ItemId</t>
   </si>
   <si>
@@ -217,6 +187,81 @@
   </si>
   <si>
     <t>Accountname</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One to many </t>
+  </si>
+  <si>
+    <t>Subscribedevents</t>
+  </si>
+  <si>
+    <t>event id</t>
+  </si>
+  <si>
+    <t>foreign key(eventid) references events(eventid)</t>
+  </si>
+  <si>
+    <t>Many to many</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psno varchar(100), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    score int, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    eventid int, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    itemid int</t>
+  </si>
+  <si>
+    <t>foreign key(psno) references users(psno),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    foreign key(eventid) references events(eventid),  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    foreign key(itemid) references items(itemid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For user to scores </t>
+  </si>
+  <si>
+    <t>one to many</t>
+  </si>
+  <si>
+    <t>for event to score</t>
+  </si>
+  <si>
+    <t>panelist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> psno varchar(100) primary key</t>
+  </si>
+  <si>
+    <t>admintable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psno </t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>varchar(100)'</t>
+  </si>
+  <si>
+    <t>foreign key references users(psno)</t>
+  </si>
+  <si>
+    <t>One to one</t>
   </si>
 </sst>
 </file>
@@ -232,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +347,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -445,6 +508,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,6 +757,237 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8717280" y="4998720"/>
+          <a:ext cx="0" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2987040" y="1272540"/>
+          <a:ext cx="2484120" cy="30480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2987040" y="1295400"/>
+          <a:ext cx="15240" cy="7284720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2994660" y="8442960"/>
+          <a:ext cx="2461260" cy="91440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10005060" y="2346960"/>
+          <a:ext cx="1234440" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1330,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J2:O51"/>
+  <dimension ref="D2:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1341,10 +1638,12 @@
     <col min="10" max="10" width="17.88671875" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" customWidth="1"/>
     <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="22" max="22" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="10:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J3" s="10"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11" t="s">
@@ -1353,21 +1652,31 @@
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="12"/>
-    </row>
-    <row r="4" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+    </row>
+    <row r="4" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J4" s="13"/>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
       <c r="O4" s="15"/>
-    </row>
-    <row r="5" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R4" s="46"/>
+      <c r="S4" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+    </row>
+    <row r="5" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J5" s="13" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L5" s="14" t="s">
         <v>28</v>
@@ -1375,52 +1684,78 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+    </row>
+    <row r="6" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J6" s="13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
-    </row>
-    <row r="7" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R6" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="U6" s="46"/>
+    </row>
+    <row r="7" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J7" s="13" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
-    </row>
-    <row r="8" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+    </row>
+    <row r="8" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J8" s="13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="15"/>
-    </row>
-    <row r="9" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+    </row>
+    <row r="9" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
-    </row>
-    <row r="10" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+    </row>
+    <row r="10" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J10" s="13"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -1428,7 +1763,7 @@
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
     </row>
-    <row r="11" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J11" s="13"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -1436,7 +1771,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
     </row>
-    <row r="12" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J12" s="13"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -1444,16 +1779,34 @@
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
     </row>
-    <row r="13" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="10:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J13" s="16"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="18"/>
-    </row>
-    <row r="15" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="P13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="R14" s="48"/>
+      <c r="S14" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+    </row>
+    <row r="15" spans="10:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+    </row>
+    <row r="16" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J16" s="19"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20" t="s">
@@ -1462,18 +1815,38 @@
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="21"/>
-    </row>
-    <row r="17" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R16" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="S16" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="T16" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+    </row>
+    <row r="17" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J17" s="22"/>
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="23"/>
       <c r="O17" s="24"/>
-    </row>
-    <row r="18" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R17" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="S17" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+    </row>
+    <row r="18" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J18" s="22" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>30</v>
@@ -1484,58 +1857,78 @@
       <c r="M18" s="23"/>
       <c r="N18" s="23"/>
       <c r="O18" s="24"/>
-    </row>
-    <row r="19" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="48"/>
+    </row>
+    <row r="19" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J19" s="22" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="L19" s="23"/>
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
       <c r="O19" s="24"/>
-    </row>
-    <row r="20" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R19" s="48"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="48"/>
+    </row>
+    <row r="20" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J20" s="22" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="K20" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L20" s="23"/>
       <c r="M20" s="23"/>
       <c r="N20" s="23"/>
       <c r="O20" s="24"/>
-    </row>
-    <row r="21" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+    </row>
+    <row r="21" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J21" s="22" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="K21" s="23" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="L21" s="23"/>
       <c r="M21" s="23"/>
       <c r="N21" s="23"/>
       <c r="O21" s="24"/>
-    </row>
-    <row r="22" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+    </row>
+    <row r="22" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J22" s="22" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="L22" s="23"/>
       <c r="M22" s="23"/>
       <c r="N22" s="23"/>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J23" s="22" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>31</v>
@@ -1545,9 +1938,9 @@
       <c r="N23" s="23"/>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J24" s="22" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="K24" s="23" t="s">
         <v>31</v>
@@ -1557,23 +1950,19 @@
       <c r="N24" s="23"/>
       <c r="O24" s="24"/>
     </row>
-    <row r="25" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J25" s="22" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="L25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="23" t="s">
-        <v>35</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
       <c r="N25" s="23"/>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J26" s="22"/>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
@@ -1581,7 +1970,7 @@
       <c r="N26" s="23"/>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J27" s="25"/>
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
@@ -1589,18 +1978,25 @@
       <c r="N27" s="26"/>
       <c r="O27" s="27"/>
     </row>
-    <row r="29" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
       <c r="J30" s="28"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="M30" s="29"/>
       <c r="N30" s="29"/>
       <c r="O30" s="30"/>
     </row>
-    <row r="31" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J31" s="31"/>
       <c r="K31" s="32"/>
       <c r="L31" s="32"/>
@@ -1608,9 +2004,9 @@
       <c r="N31" s="32"/>
       <c r="O31" s="33"/>
     </row>
-    <row r="32" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:22" x14ac:dyDescent="0.3">
       <c r="J32" s="31" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K32" s="32" t="s">
         <v>27</v>
@@ -1624,10 +2020,10 @@
     </row>
     <row r="33" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J33" s="31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K33" s="32" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="L33" s="32"/>
       <c r="M33" s="32"/>
@@ -1636,7 +2032,7 @@
     </row>
     <row r="34" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J34" s="31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K34" s="32" t="s">
         <v>31</v>
@@ -1648,13 +2044,13 @@
     </row>
     <row r="35" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J35" s="31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K35" s="32" t="s">
         <v>27</v>
       </c>
       <c r="L35" s="32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M35" s="32"/>
       <c r="N35" s="32"/>
@@ -1697,7 +2093,7 @@
       <c r="J42" s="37"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="M42" s="38"/>
       <c r="N42" s="38"/>
@@ -1713,13 +2109,13 @@
     </row>
     <row r="44" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J44" s="40" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K44" s="41" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="L44" s="41" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M44" s="41"/>
       <c r="N44" s="41"/>
@@ -1727,28 +2123,22 @@
     </row>
     <row r="45" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J45" s="40" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="K45" s="41" t="s">
         <v>27</v>
       </c>
       <c r="L45" s="41" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="M45" s="41"/>
       <c r="N45" s="41"/>
       <c r="O45" s="42"/>
     </row>
     <row r="46" spans="10:15" x14ac:dyDescent="0.3">
-      <c r="J46" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="K46" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="L46" s="41" t="s">
-        <v>46</v>
-      </c>
+      <c r="J46" s="40"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
       <c r="M46" s="41"/>
       <c r="N46" s="41"/>
       <c r="O46" s="42"/>
@@ -1769,7 +2159,7 @@
       <c r="N48" s="41"/>
       <c r="O48" s="42"/>
     </row>
-    <row r="49" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J49" s="40"/>
       <c r="K49" s="41"/>
       <c r="L49" s="41"/>
@@ -1777,7 +2167,7 @@
       <c r="N49" s="41"/>
       <c r="O49" s="42"/>
     </row>
-    <row r="50" spans="10:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J50" s="40"/>
       <c r="K50" s="41"/>
       <c r="L50" s="41"/>
@@ -1785,7 +2175,7 @@
       <c r="N50" s="41"/>
       <c r="O50" s="42"/>
     </row>
-    <row r="51" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J51" s="43"/>
       <c r="K51" s="44"/>
       <c r="L51" s="44"/>
@@ -1793,7 +2183,189 @@
       <c r="N51" s="44"/>
       <c r="O51" s="45"/>
     </row>
+    <row r="54" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J54" s="47"/>
+      <c r="K54" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="L54" s="47"/>
+      <c r="M54" s="47"/>
+      <c r="N54" s="47"/>
+    </row>
+    <row r="55" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="47"/>
+      <c r="N55" s="47"/>
+    </row>
+    <row r="56" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J56" s="47"/>
+      <c r="K56" s="47"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="47"/>
+      <c r="O56" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J57" s="47"/>
+      <c r="K57" s="47"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="47"/>
+      <c r="N57" s="47"/>
+    </row>
+    <row r="58" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="47"/>
+      <c r="N58" s="47"/>
+      <c r="O58" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J59" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="K59" s="47"/>
+      <c r="L59" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="M59" s="47"/>
+      <c r="N59" s="47"/>
+    </row>
+    <row r="60" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J60" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K60" s="47"/>
+      <c r="L60" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="M60" s="47"/>
+      <c r="N60" s="47"/>
+    </row>
+    <row r="61" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J61" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="K61" s="47"/>
+      <c r="L61" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="M61" s="47"/>
+      <c r="N61" s="47"/>
+    </row>
+    <row r="62" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J62" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="K62" s="47"/>
+      <c r="L62" s="47"/>
+      <c r="M62" s="47"/>
+      <c r="N62" s="47"/>
+    </row>
+    <row r="63" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J63" s="47"/>
+      <c r="K63" s="47"/>
+      <c r="L63" s="47"/>
+      <c r="M63" s="47"/>
+      <c r="N63" s="47"/>
+    </row>
+    <row r="64" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J64" s="47"/>
+      <c r="K64" s="47"/>
+      <c r="L64" s="47"/>
+      <c r="M64" s="47"/>
+      <c r="N64" s="47"/>
+    </row>
+    <row r="65" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J65" s="47"/>
+      <c r="K65" s="47"/>
+      <c r="L65" s="47"/>
+      <c r="M65" s="47"/>
+      <c r="N65" s="47"/>
+    </row>
+    <row r="66" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J66" s="47"/>
+      <c r="K66" s="47"/>
+      <c r="L66" s="47"/>
+      <c r="M66" s="47"/>
+      <c r="N66" s="47"/>
+    </row>
+    <row r="67" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J67" s="47"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="47"/>
+      <c r="M67" s="47"/>
+      <c r="N67" s="47"/>
+    </row>
+    <row r="68" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J68" s="47"/>
+      <c r="K68" s="47"/>
+      <c r="L68" s="47"/>
+      <c r="M68" s="47"/>
+      <c r="N68" s="47"/>
+    </row>
+    <row r="72" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Seventh commit 21 april 11.30am
</commit_message>
<xml_diff>
--- a/Project Flow.xlsx
+++ b/Project Flow.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t xml:space="preserve">Login Page </t>
   </si>
@@ -243,9 +243,6 @@
     <t>panelist</t>
   </si>
   <si>
-    <t xml:space="preserve"> psno varchar(100) primary key</t>
-  </si>
-  <si>
     <t>admintable</t>
   </si>
   <si>
@@ -262,6 +259,30 @@
   </si>
   <si>
     <t>One to one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logintime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">logouttime </t>
+  </si>
+  <si>
+    <t>loginflag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eventid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign key references users(psno) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign key references events(eventid) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoredate </t>
+  </si>
+  <si>
+    <t>scoretime</t>
   </si>
 </sst>
 </file>
@@ -996,6 +1017,53 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10012680" y="1706880"/>
+          <a:ext cx="1905000" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1630,7 +1698,7 @@
   <dimension ref="D2:V79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,10 +1772,10 @@
         <v>45</v>
       </c>
       <c r="S6" s="46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T6" s="46" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="U6" s="46"/>
     </row>
@@ -1722,9 +1790,15 @@
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
-      <c r="R7" s="46"/>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
+      <c r="R7" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7" s="46" t="s">
+        <v>83</v>
+      </c>
       <c r="U7" s="46"/>
     </row>
     <row r="8" spans="10:22" x14ac:dyDescent="0.3">
@@ -1744,8 +1818,12 @@
       <c r="U8" s="46"/>
     </row>
     <row r="9" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
+      <c r="J9" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
@@ -1756,20 +1834,31 @@
       <c r="U9" s="46"/>
     </row>
     <row r="10" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
+      <c r="J10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="10:22" x14ac:dyDescent="0.3">
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
+      <c r="J11" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
+      <c r="S11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="10:22" x14ac:dyDescent="0.3">
       <c r="J12" s="13"/>
@@ -1787,13 +1876,13 @@
       <c r="N13" s="17"/>
       <c r="O13" s="18"/>
       <c r="P13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="10:22" x14ac:dyDescent="0.3">
       <c r="R14" s="48"/>
       <c r="S14" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T14" s="48"/>
       <c r="U14" s="48"/>
@@ -1816,13 +1905,13 @@
       <c r="N16" s="20"/>
       <c r="O16" s="21"/>
       <c r="R16" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S16" s="48" t="s">
         <v>40</v>
       </c>
       <c r="T16" s="48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U16" s="48"/>
       <c r="V16" s="48"/>
@@ -1835,7 +1924,7 @@
       <c r="N17" s="23"/>
       <c r="O17" s="24"/>
       <c r="R17" s="48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S17" s="48" t="s">
         <v>40</v>
@@ -2275,15 +2364,23 @@
       <c r="N62" s="47"/>
     </row>
     <row r="63" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J63" s="47"/>
-      <c r="K63" s="47"/>
+      <c r="J63" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="K63" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="L63" s="47"/>
       <c r="M63" s="47"/>
       <c r="N63" s="47"/>
     </row>
     <row r="64" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J64" s="47"/>
-      <c r="K64" s="47"/>
+      <c r="J64" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="K64" s="47" t="s">
+        <v>54</v>
+      </c>
       <c r="L64" s="47"/>
       <c r="M64" s="47"/>
       <c r="N64" s="47"/>

</xml_diff>